<commit_message>
Update BOM, load updated PCB files for target
</commit_message>
<xml_diff>
--- a/hardware/targets/ztex/pcb/ztex_openadc_eagle/bom_openadc_ztex.xlsx
+++ b/hardware/targets/ztex/pcb/ztex_openadc_eagle/bom_openadc_ztex.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="398">
   <si>
     <t>587-2100-1-ND</t>
   </si>
@@ -1256,6 +1256,15 @@
   </si>
   <si>
     <t>BAV99-FDICT-ND</t>
+  </si>
+  <si>
+    <t>A33184-ND</t>
+  </si>
+  <si>
+    <t>A106446-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A26494-ND </t>
   </si>
 </sst>
 </file>
@@ -2999,10 +3008,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B51"/>
+  <dimension ref="A1:B53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A45" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3011,6 +3020,14 @@
     <col min="5" max="5" width="69" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>395</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
@@ -3409,6 +3426,22 @@
       </c>
       <c r="B51" t="s">
         <v>394</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>397</v>
       </c>
     </row>
   </sheetData>

</xml_diff>